<commit_message>
Updates to list of priorities
</commit_message>
<xml_diff>
--- a/List_of_priorities.xlsx
+++ b/List_of_priorities.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t xml:space="preserve">List of priorities </t>
   </si>
@@ -96,6 +96,48 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kat </t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Lines </t>
+  </si>
+  <si>
+    <t>Colored Boxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changing tools </t>
+  </si>
+  <si>
+    <t>Changing Tools</t>
+  </si>
+  <si>
+    <t>add segments to existing lines</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Lightweight STL editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uploading data </t>
+  </si>
+  <si>
+    <t>Upload data to graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High </t>
   </si>
 </sst>
 </file>
@@ -428,16 +470,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E13"/>
+  <dimension ref="A2:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.21875" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
     <col min="3" max="3" width="66.109375" customWidth="1"/>
     <col min="4" max="4" width="35.6640625" customWidth="1"/>
   </cols>
@@ -580,6 +622,75 @@
         <v>20</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>